<commit_message>
tra compare with ref
</commit_message>
<xml_diff>
--- a/Data/selected_features/features_of_interest.xlsx
+++ b/Data/selected_features/features_of_interest.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PlasmaEV_GBMVsHC" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="UrineEV_GBMVsHC" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Reference" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SerumExosome_GBMVsHC" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Reference" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="314">
   <si>
     <t xml:space="preserve">Protein</t>
   </si>
@@ -843,6 +844,87 @@
     <t xml:space="preserve">CLIC1</t>
   </si>
   <si>
+    <t xml:space="preserve">miRNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-486-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-182-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-486-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-378a-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-183-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-501-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-20b-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-106b-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-629-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-185-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-25-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-21-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-let-7a-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-381-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-409-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-let-7d-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-323b-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-328-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-339-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-340-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-126-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-130b-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-493-5p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-654-3p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsa-miR-485-3p</t>
+  </si>
+  <si>
     <t xml:space="preserve">SheetName</t>
   </si>
   <si>
@@ -862,6 +944,24 @@
   </si>
   <si>
     <t xml:space="preserve">IDH-wt GBM vs  Healthy + non-glioma controls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.3390/ijms21134754 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UrineEV_GBMVsHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBM diagnostic : GBM Pre-op vs Healthy controls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper under review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SerumExosome_GBMVsHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBM Vs Healthy</t>
   </si>
   <si>
     <r>
@@ -872,7 +972,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://doi.org/10.3390/ijms21134754</t>
+      <t xml:space="preserve">https://doi.org/10.1038/s41698-018-0071-0</t>
     </r>
     <r>
       <rPr>
@@ -884,15 +984,6 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
-  <si>
-    <t xml:space="preserve">UrineEV_GBMVsHC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBM diagnostic : GBM Pre-op vs Healthy controls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paper under review</t>
-  </si>
 </sst>
 </file>
 
@@ -901,7 +992,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -925,6 +1016,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -980,7 +1079,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -993,7 +1092,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1016,7 +1135,7 @@
   </sheetPr>
   <dimension ref="A1:A69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2463,10 +2582,416 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:J27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="23.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2475,58 +3000,73 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="56.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>273</v>
+        <v>300</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>275</v>
+        <v>302</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>276</v>
+        <v>303</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>280</v>
+        <v>306</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>282</v>
+        <v>309</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>283</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://doi.org/10.3390/ijms21134754"/>
+    <hyperlink ref="D2" r:id="rId1" display="https://doi.org/10.3390/ijms21134754 "/>
+    <hyperlink ref="D4" r:id="rId2" display="https://doi.org/10.1038/s41698-018-0071-0"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>